<commit_message>
use exact municipalities of B-C for did_reg regressions when bal_48==1
</commit_message>
<xml_diff>
--- a/Tables/did_reg_emp.xlsx
+++ b/Tables/did_reg_emp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50165415-9575-430C-BB7B-C99F7899930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8060F99D-6308-4D93-8CBC-F6ED9D255683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{83DCEEBE-B711-4EA6-8CCA-AE15FFD6ECFA}"/>
+    <workbookView xWindow="-28920" yWindow="-8190" windowWidth="29040" windowHeight="15720" xr2:uid="{83DCEEBE-B711-4EA6-8CCA-AE15FFD6ECFA}"/>
   </bookViews>
   <sheets>
     <sheet name="did_reg_emp" sheetId="1" r:id="rId1"/>
@@ -256,28 +256,28 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-0.069***</v>
+            <v>-0.066***</v>
           </cell>
           <cell r="C5" t="str">
             <v>-0.046***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-0.00034</v>
+            <v>-0.00020</v>
           </cell>
           <cell r="E5" t="str">
             <v>0.0012</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-0.016</v>
+            <v>-0.017</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.0031</v>
+            <v>-0.0029</v>
           </cell>
           <cell r="H5" t="str">
             <v>-0.019</v>
           </cell>
           <cell r="I5" t="str">
-            <v>0.0087</v>
+            <v>0.0086</v>
           </cell>
           <cell r="J5" t="str">
             <v>-0.12**</v>
@@ -320,19 +320,19 @@
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>-0.044***</v>
+            <v>-0.042***</v>
           </cell>
           <cell r="C8" t="str">
             <v>-0.036***</v>
           </cell>
           <cell r="D8" t="str">
-            <v>-0.0053</v>
+            <v>-0.0052</v>
           </cell>
           <cell r="E8" t="str">
-            <v>-0.0091</v>
+            <v>-0.0090</v>
           </cell>
           <cell r="F8" t="str">
-            <v>-0.0094</v>
+            <v>-0.0095</v>
           </cell>
           <cell r="G8" t="str">
             <v>-0.0051</v>
@@ -352,7 +352,7 @@
         </row>
         <row r="9">
           <cell r="B9" t="str">
-            <v>(0.012)</v>
+            <v>(0.011)</v>
           </cell>
           <cell r="C9" t="str">
             <v>(0.011)</v>
@@ -384,22 +384,22 @@
         </row>
         <row r="11">
           <cell r="B11" t="str">
-            <v>-0.019***</v>
+            <v>-0.018***</v>
           </cell>
           <cell r="C11" t="str">
             <v>-0.015**</v>
           </cell>
           <cell r="D11" t="str">
-            <v>-0.0028</v>
+            <v>-0.0030</v>
           </cell>
           <cell r="E11" t="str">
-            <v>-0.0054</v>
+            <v>-0.0057</v>
           </cell>
           <cell r="F11" t="str">
-            <v>-0.0018</v>
+            <v>-0.0019</v>
           </cell>
           <cell r="G11" t="str">
-            <v>0.0011</v>
+            <v>0.0012</v>
           </cell>
           <cell r="H11" t="str">
             <v>-0.0034</v>
@@ -416,7 +416,7 @@
         </row>
         <row r="12">
           <cell r="B12" t="str">
-            <v>(0.0062)</v>
+            <v>(0.0061)</v>
           </cell>
           <cell r="C12" t="str">
             <v>(0.0061)</v>
@@ -448,25 +448,25 @@
         </row>
         <row r="14">
           <cell r="B14" t="str">
-            <v>0.015***</v>
+            <v>0.014***</v>
           </cell>
           <cell r="C14" t="str">
             <v>0.011**</v>
           </cell>
           <cell r="D14" t="str">
-            <v>-0.0094**</v>
+            <v>-0.0096**</v>
           </cell>
           <cell r="E14" t="str">
-            <v>-0.0067</v>
+            <v>-0.0069</v>
           </cell>
           <cell r="F14" t="str">
-            <v>-0.0015</v>
+            <v>-0.0018</v>
           </cell>
           <cell r="G14" t="str">
-            <v>-0.0012</v>
+            <v>-0.0017</v>
           </cell>
           <cell r="H14" t="str">
-            <v>-0.0024</v>
+            <v>-0.0023</v>
           </cell>
           <cell r="I14" t="str">
             <v>-0.0089</v>
@@ -483,7 +483,7 @@
             <v>(0.0050)</v>
           </cell>
           <cell r="C15" t="str">
-            <v>(0.0051)</v>
+            <v>(0.0050)</v>
           </cell>
           <cell r="D15" t="str">
             <v>(0.0046)</v>
@@ -515,19 +515,19 @@
             <v>0.024***</v>
           </cell>
           <cell r="C17" t="str">
-            <v>0.022***</v>
+            <v>0.023***</v>
           </cell>
           <cell r="D17" t="str">
             <v>-0.015**</v>
           </cell>
           <cell r="E17" t="str">
-            <v>-0.0070</v>
+            <v>-0.0072</v>
           </cell>
           <cell r="F17" t="str">
             <v>-0.0068</v>
           </cell>
           <cell r="G17" t="str">
-            <v>-0.0033</v>
+            <v>-0.0036</v>
           </cell>
           <cell r="H17" t="str">
             <v>-0.0019</v>
@@ -544,10 +544,10 @@
         </row>
         <row r="18">
           <cell r="B18" t="str">
-            <v>(0.0091)</v>
+            <v>(0.0090)</v>
           </cell>
           <cell r="C18" t="str">
-            <v>(0.0087)</v>
+            <v>(0.0085)</v>
           </cell>
           <cell r="D18" t="str">
             <v>(0.0074)</v>
@@ -556,7 +556,7 @@
             <v>(0.0074)</v>
           </cell>
           <cell r="F18" t="str">
-            <v>(0.0065)</v>
+            <v>(0.0066)</v>
           </cell>
           <cell r="G18" t="str">
             <v>(0.0062)</v>
@@ -576,25 +576,25 @@
         </row>
         <row r="20">
           <cell r="B20" t="str">
-            <v>0.025**</v>
+            <v>0.027**</v>
           </cell>
           <cell r="C20" t="str">
-            <v>0.028**</v>
+            <v>0.029***</v>
           </cell>
           <cell r="D20" t="str">
             <v>-0.022**</v>
           </cell>
           <cell r="E20" t="str">
-            <v>-0.0093</v>
+            <v>-0.0095</v>
           </cell>
           <cell r="F20" t="str">
-            <v>-0.013</v>
+            <v>-0.012</v>
           </cell>
           <cell r="G20" t="str">
-            <v>-0.0063</v>
+            <v>-0.0058</v>
           </cell>
           <cell r="H20" t="str">
-            <v>0.00026</v>
+            <v>0.00025</v>
           </cell>
           <cell r="I20" t="str">
             <v>-0.0043</v>
@@ -640,16 +640,16 @@
         </row>
         <row r="23">
           <cell r="B23" t="str">
-            <v>0.017</v>
+            <v>0.019</v>
           </cell>
           <cell r="C23" t="str">
-            <v>0.022</v>
+            <v>0.024*</v>
           </cell>
           <cell r="D23" t="str">
-            <v>-0.026**</v>
+            <v>-0.027**</v>
           </cell>
           <cell r="E23" t="str">
-            <v>-0.0095</v>
+            <v>-0.0098</v>
           </cell>
           <cell r="F23" t="str">
             <v>-0.022**</v>
@@ -658,7 +658,7 @@
             <v>-0.013</v>
           </cell>
           <cell r="H23" t="str">
-            <v>0.000070</v>
+            <v>0.000078</v>
           </cell>
           <cell r="I23" t="str">
             <v>-0.0038</v>
@@ -672,7 +672,7 @@
         </row>
         <row r="24">
           <cell r="B24" t="str">
-            <v>(0.016)</v>
+            <v>(0.015)</v>
           </cell>
           <cell r="C24" t="str">
             <v>(0.014)</v>
@@ -704,22 +704,22 @@
         </row>
         <row r="26">
           <cell r="B26" t="str">
-            <v>0.00011</v>
+            <v>0.0059</v>
           </cell>
           <cell r="C26" t="str">
-            <v>0.023</v>
+            <v>0.026</v>
           </cell>
           <cell r="D26" t="str">
-            <v>-0.038**</v>
+            <v>-0.039***</v>
           </cell>
           <cell r="E26" t="str">
-            <v>-0.0090</v>
+            <v>-0.0093</v>
           </cell>
           <cell r="F26" t="str">
-            <v>-0.036***</v>
+            <v>-0.035***</v>
           </cell>
           <cell r="G26" t="str">
-            <v>-0.015</v>
+            <v>-0.014</v>
           </cell>
           <cell r="H26" t="str">
             <v>-0.024</v>
@@ -739,10 +739,10 @@
             <v/>
           </cell>
           <cell r="B27" t="str">
-            <v>(0.020)</v>
+            <v>(0.019)</v>
           </cell>
           <cell r="C27" t="str">
-            <v>(0.017)</v>
+            <v>(0.016)</v>
           </cell>
           <cell r="D27" t="str">
             <v>(0.015)</v>
@@ -771,28 +771,28 @@
         </row>
         <row r="29">
           <cell r="B29" t="str">
-            <v>66268</v>
+            <v>65424</v>
           </cell>
           <cell r="C29" t="str">
-            <v>66127</v>
+            <v>65283</v>
           </cell>
           <cell r="D29" t="str">
-            <v>64223</v>
+            <v>63586</v>
           </cell>
           <cell r="E29" t="str">
-            <v>64082</v>
+            <v>63445</v>
           </cell>
           <cell r="F29" t="str">
-            <v>65802</v>
+            <v>65200</v>
           </cell>
           <cell r="G29" t="str">
-            <v>65661</v>
+            <v>65059</v>
           </cell>
           <cell r="H29" t="str">
-            <v>42849</v>
+            <v>42839</v>
           </cell>
           <cell r="I29" t="str">
-            <v>42708</v>
+            <v>42698</v>
           </cell>
           <cell r="J29" t="str">
             <v>24402</v>
@@ -806,22 +806,22 @@
             <v>R-sq</v>
           </cell>
           <cell r="B30" t="str">
-            <v>0.221</v>
+            <v>0.229</v>
           </cell>
           <cell r="C30" t="str">
-            <v>0.233</v>
+            <v>0.240</v>
           </cell>
           <cell r="D30" t="str">
-            <v>0.186</v>
+            <v>0.188</v>
           </cell>
           <cell r="E30" t="str">
-            <v>0.193</v>
+            <v>0.195</v>
           </cell>
           <cell r="F30" t="str">
-            <v>0.193</v>
+            <v>0.198</v>
           </cell>
           <cell r="G30" t="str">
-            <v>0.204</v>
+            <v>0.210</v>
           </cell>
           <cell r="H30" t="str">
             <v>0.270</v>
@@ -841,22 +841,22 @@
             <v>DepVarMean</v>
           </cell>
           <cell r="B31" t="str">
-            <v>6.33</v>
+            <v>6.39</v>
           </cell>
           <cell r="C31" t="str">
-            <v>6.32</v>
+            <v>6.38</v>
           </cell>
           <cell r="D31" t="str">
-            <v>3.18</v>
+            <v>3.21</v>
           </cell>
           <cell r="E31" t="str">
-            <v>3.17</v>
+            <v>3.20</v>
           </cell>
           <cell r="F31" t="str">
-            <v>5.56</v>
+            <v>5.59</v>
           </cell>
           <cell r="G31" t="str">
-            <v>5.55</v>
+            <v>5.58</v>
           </cell>
           <cell r="H31" t="str">
             <v>6.19</v>
@@ -873,28 +873,28 @@
         </row>
         <row r="32">
           <cell r="B32" t="str">
-            <v>1410</v>
+            <v>1392</v>
           </cell>
           <cell r="C32" t="str">
-            <v>1407</v>
+            <v>1389</v>
           </cell>
           <cell r="D32" t="str">
-            <v>1410</v>
+            <v>1392</v>
           </cell>
           <cell r="E32" t="str">
-            <v>1407</v>
+            <v>1389</v>
           </cell>
           <cell r="F32" t="str">
-            <v>1410</v>
+            <v>1392</v>
           </cell>
           <cell r="G32" t="str">
-            <v>1407</v>
+            <v>1389</v>
           </cell>
           <cell r="H32" t="str">
-            <v>1208</v>
+            <v>1205</v>
           </cell>
           <cell r="I32" t="str">
-            <v>1205</v>
+            <v>1202</v>
           </cell>
           <cell r="J32" t="str">
             <v>764</v>
@@ -905,13 +905,13 @@
         </row>
         <row r="33">
           <cell r="C33" t="str">
-            <v>0.00074</v>
+            <v>0.00059</v>
           </cell>
           <cell r="E33" t="str">
-            <v>2.1e-11</v>
+            <v>1.6e-11</v>
           </cell>
           <cell r="G33" t="str">
-            <v>0.0020</v>
+            <v>0.0014</v>
           </cell>
           <cell r="I33" t="str">
             <v>0.00067</v>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>[1]did_reg_emp!B5</f>
-        <v>-0.069***</v>
+        <v>-0.066***</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>[1]did_reg_emp!C5</f>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="E5" s="3" t="str">
         <f>[1]did_reg_emp!D5</f>
-        <v>-0.00034</v>
+        <v>-0.00020</v>
       </c>
       <c r="F5" s="3" t="str">
         <f>[1]did_reg_emp!E5</f>
@@ -1370,11 +1370,11 @@
       </c>
       <c r="H5" s="3" t="str">
         <f>[1]did_reg_emp!F5</f>
-        <v>-0.016</v>
+        <v>-0.017</v>
       </c>
       <c r="I5" s="3" t="str">
         <f>[1]did_reg_emp!G5</f>
-        <v>-0.0031</v>
+        <v>-0.0029</v>
       </c>
       <c r="K5" s="3" t="str">
         <f>[1]did_reg_emp!H5</f>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="L5" s="3" t="str">
         <f>[1]did_reg_emp!I5</f>
-        <v>0.0087</v>
+        <v>0.0086</v>
       </c>
       <c r="N5" s="3" t="str">
         <f>[1]did_reg_emp!J5</f>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f>[1]did_reg_emp!B8</f>
-        <v>-0.044***</v>
+        <v>-0.042***</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>[1]did_reg_emp!C8</f>
@@ -1449,15 +1449,15 @@
       </c>
       <c r="E7" s="3" t="str">
         <f>[1]did_reg_emp!D8</f>
-        <v>-0.0053</v>
+        <v>-0.0052</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>[1]did_reg_emp!E8</f>
-        <v>-0.0091</v>
+        <v>-0.0090</v>
       </c>
       <c r="H7" s="3" t="str">
         <f>[1]did_reg_emp!F8</f>
-        <v>-0.0094</v>
+        <v>-0.0095</v>
       </c>
       <c r="I7" s="3" t="str">
         <f>[1]did_reg_emp!G8</f>
@@ -1483,7 +1483,7 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="str">
         <f>[1]did_reg_emp!B9</f>
-        <v>(0.012)</v>
+        <v>(0.011)</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>[1]did_reg_emp!C9</f>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f>[1]did_reg_emp!B11</f>
-        <v>-0.019***</v>
+        <v>-0.018***</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>[1]did_reg_emp!C11</f>
@@ -1536,19 +1536,19 @@
       </c>
       <c r="E9" s="3" t="str">
         <f>[1]did_reg_emp!D11</f>
-        <v>-0.0028</v>
+        <v>-0.0030</v>
       </c>
       <c r="F9" s="3" t="str">
         <f>[1]did_reg_emp!E11</f>
-        <v>-0.0054</v>
+        <v>-0.0057</v>
       </c>
       <c r="H9" s="3" t="str">
         <f>[1]did_reg_emp!F11</f>
-        <v>-0.0018</v>
+        <v>-0.0019</v>
       </c>
       <c r="I9" s="3" t="str">
         <f>[1]did_reg_emp!G11</f>
-        <v>0.0011</v>
+        <v>0.0012</v>
       </c>
       <c r="K9" s="3" t="str">
         <f>[1]did_reg_emp!H11</f>
@@ -1570,7 +1570,7 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="str">
         <f>[1]did_reg_emp!B12</f>
-        <v>(0.0062)</v>
+        <v>(0.0061)</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>[1]did_reg_emp!C12</f>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>[1]did_reg_emp!B14</f>
-        <v>0.015***</v>
+        <v>0.014***</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>[1]did_reg_emp!C14</f>
@@ -1623,23 +1623,23 @@
       </c>
       <c r="E12" s="3" t="str">
         <f>[1]did_reg_emp!D14</f>
-        <v>-0.0094**</v>
+        <v>-0.0096**</v>
       </c>
       <c r="F12" s="3" t="str">
         <f>[1]did_reg_emp!E14</f>
-        <v>-0.0067</v>
+        <v>-0.0069</v>
       </c>
       <c r="H12" s="3" t="str">
         <f>[1]did_reg_emp!F14</f>
-        <v>-0.0015</v>
+        <v>-0.0018</v>
       </c>
       <c r="I12" s="3" t="str">
         <f>[1]did_reg_emp!G14</f>
-        <v>-0.0012</v>
+        <v>-0.0017</v>
       </c>
       <c r="K12" s="3" t="str">
         <f>[1]did_reg_emp!H14</f>
-        <v>-0.0024</v>
+        <v>-0.0023</v>
       </c>
       <c r="L12" s="3" t="str">
         <f>[1]did_reg_emp!I14</f>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C13" s="3" t="str">
         <f>[1]did_reg_emp!C15</f>
-        <v>(0.0051)</v>
+        <v>(0.0050)</v>
       </c>
       <c r="E13" s="3" t="str">
         <f>[1]did_reg_emp!D15</f>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C14" s="3" t="str">
         <f>[1]did_reg_emp!C17</f>
-        <v>0.022***</v>
+        <v>0.023***</v>
       </c>
       <c r="E14" s="3" t="str">
         <f>[1]did_reg_emp!D17</f>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="F14" s="3" t="str">
         <f>[1]did_reg_emp!E17</f>
-        <v>-0.0070</v>
+        <v>-0.0072</v>
       </c>
       <c r="H14" s="3" t="str">
         <f>[1]did_reg_emp!F17</f>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="I14" s="3" t="str">
         <f>[1]did_reg_emp!G17</f>
-        <v>-0.0033</v>
+        <v>-0.0036</v>
       </c>
       <c r="K14" s="3" t="str">
         <f>[1]did_reg_emp!H17</f>
@@ -1744,11 +1744,11 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f>[1]did_reg_emp!B18</f>
-        <v>(0.0091)</v>
+        <v>(0.0090)</v>
       </c>
       <c r="C15" s="3" t="str">
         <f>[1]did_reg_emp!C18</f>
-        <v>(0.0087)</v>
+        <v>(0.0085)</v>
       </c>
       <c r="E15" s="3" t="str">
         <f>[1]did_reg_emp!D18</f>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="H15" s="3" t="str">
         <f>[1]did_reg_emp!F18</f>
-        <v>(0.0065)</v>
+        <v>(0.0066)</v>
       </c>
       <c r="I15" s="3" t="str">
         <f>[1]did_reg_emp!G18</f>
@@ -1789,11 +1789,11 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>[1]did_reg_emp!B20</f>
-        <v>0.025**</v>
+        <v>0.027**</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>[1]did_reg_emp!C20</f>
-        <v>0.028**</v>
+        <v>0.029***</v>
       </c>
       <c r="E16" s="3" t="str">
         <f>[1]did_reg_emp!D20</f>
@@ -1801,19 +1801,19 @@
       </c>
       <c r="F16" s="3" t="str">
         <f>[1]did_reg_emp!E20</f>
-        <v>-0.0093</v>
+        <v>-0.0095</v>
       </c>
       <c r="H16" s="3" t="str">
         <f>[1]did_reg_emp!F20</f>
-        <v>-0.013</v>
+        <v>-0.012</v>
       </c>
       <c r="I16" s="3" t="str">
         <f>[1]did_reg_emp!G20</f>
-        <v>-0.0063</v>
+        <v>-0.0058</v>
       </c>
       <c r="K16" s="3" t="str">
         <f>[1]did_reg_emp!H20</f>
-        <v>0.00026</v>
+        <v>0.00025</v>
       </c>
       <c r="L16" s="3" t="str">
         <f>[1]did_reg_emp!I20</f>
@@ -1876,19 +1876,19 @@
       </c>
       <c r="B18" s="3" t="str">
         <f>[1]did_reg_emp!B23</f>
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>[1]did_reg_emp!C23</f>
-        <v>0.022</v>
+        <v>0.024*</v>
       </c>
       <c r="E18" s="3" t="str">
         <f>[1]did_reg_emp!D23</f>
-        <v>-0.026**</v>
+        <v>-0.027**</v>
       </c>
       <c r="F18" s="3" t="str">
         <f>[1]did_reg_emp!E23</f>
-        <v>-0.0095</v>
+        <v>-0.0098</v>
       </c>
       <c r="H18" s="3" t="str">
         <f>[1]did_reg_emp!F23</f>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="K18" s="3" t="str">
         <f>[1]did_reg_emp!H23</f>
-        <v>0.000070</v>
+        <v>0.000078</v>
       </c>
       <c r="L18" s="3" t="str">
         <f>[1]did_reg_emp!I23</f>
@@ -1918,7 +1918,7 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="str">
         <f>[1]did_reg_emp!B24</f>
-        <v>(0.016)</v>
+        <v>(0.015)</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>[1]did_reg_emp!C24</f>
@@ -1963,27 +1963,27 @@
       </c>
       <c r="B20" s="3" t="str">
         <f>[1]did_reg_emp!B26</f>
-        <v>0.00011</v>
+        <v>0.0059</v>
       </c>
       <c r="C20" s="3" t="str">
         <f>[1]did_reg_emp!C26</f>
-        <v>0.023</v>
+        <v>0.026</v>
       </c>
       <c r="E20" s="3" t="str">
         <f>[1]did_reg_emp!D26</f>
-        <v>-0.038**</v>
+        <v>-0.039***</v>
       </c>
       <c r="F20" s="3" t="str">
         <f>[1]did_reg_emp!E26</f>
-        <v>-0.0090</v>
+        <v>-0.0093</v>
       </c>
       <c r="H20" s="3" t="str">
         <f>[1]did_reg_emp!F26</f>
-        <v>-0.036***</v>
+        <v>-0.035***</v>
       </c>
       <c r="I20" s="3" t="str">
         <f>[1]did_reg_emp!G26</f>
-        <v>-0.015</v>
+        <v>-0.014</v>
       </c>
       <c r="K20" s="3" t="str">
         <f>[1]did_reg_emp!H26</f>
@@ -2009,11 +2009,11 @@
       </c>
       <c r="B21" s="3" t="str">
         <f>[1]did_reg_emp!B27</f>
-        <v>(0.020)</v>
+        <v>(0.019)</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>[1]did_reg_emp!C27</f>
-        <v>(0.017)</v>
+        <v>(0.016)</v>
       </c>
       <c r="E21" s="3" t="str">
         <f>[1]did_reg_emp!D27</f>
@@ -2054,38 +2054,38 @@
       </c>
       <c r="B23" s="5" t="str">
         <f>[1]did_reg_emp!B29</f>
-        <v>66268</v>
+        <v>65424</v>
       </c>
       <c r="C23" s="5" t="str">
         <f>[1]did_reg_emp!C29</f>
-        <v>66127</v>
+        <v>65283</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="str">
         <f>[1]did_reg_emp!D29</f>
-        <v>64223</v>
+        <v>63586</v>
       </c>
       <c r="F23" s="5" t="str">
         <f>[1]did_reg_emp!E29</f>
-        <v>64082</v>
+        <v>63445</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="str">
         <f>[1]did_reg_emp!F29</f>
-        <v>65802</v>
+        <v>65200</v>
       </c>
       <c r="I23" s="5" t="str">
         <f>[1]did_reg_emp!G29</f>
-        <v>65661</v>
+        <v>65059</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="str">
         <f>[1]did_reg_emp!H29</f>
-        <v>42849</v>
+        <v>42839</v>
       </c>
       <c r="L23" s="5" t="str">
         <f>[1]did_reg_emp!I29</f>
-        <v>42708</v>
+        <v>42698</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5" t="str">
@@ -2103,35 +2103,35 @@
       </c>
       <c r="B24" s="3" t="str">
         <f>[1]did_reg_emp!B32</f>
-        <v>1410</v>
+        <v>1392</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>[1]did_reg_emp!C32</f>
-        <v>1407</v>
+        <v>1389</v>
       </c>
       <c r="E24" s="3" t="str">
         <f>[1]did_reg_emp!D32</f>
-        <v>1410</v>
+        <v>1392</v>
       </c>
       <c r="F24" s="3" t="str">
         <f>[1]did_reg_emp!E32</f>
-        <v>1407</v>
+        <v>1389</v>
       </c>
       <c r="H24" s="3" t="str">
         <f>[1]did_reg_emp!F32</f>
-        <v>1410</v>
+        <v>1392</v>
       </c>
       <c r="I24" s="3" t="str">
         <f>[1]did_reg_emp!G32</f>
-        <v>1407</v>
+        <v>1389</v>
       </c>
       <c r="K24" s="3" t="str">
         <f>[1]did_reg_emp!H32</f>
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="L24" s="3" t="str">
         <f>[1]did_reg_emp!I32</f>
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="N24" s="3" t="str">
         <f>[1]did_reg_emp!J32</f>
@@ -2149,27 +2149,27 @@
       </c>
       <c r="B25" s="3" t="str">
         <f>[1]did_reg_emp!B30</f>
-        <v>0.221</v>
+        <v>0.229</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>[1]did_reg_emp!C30</f>
-        <v>0.233</v>
+        <v>0.240</v>
       </c>
       <c r="E25" s="3" t="str">
         <f>[1]did_reg_emp!D30</f>
-        <v>0.186</v>
+        <v>0.188</v>
       </c>
       <c r="F25" s="3" t="str">
         <f>[1]did_reg_emp!E30</f>
-        <v>0.193</v>
+        <v>0.195</v>
       </c>
       <c r="H25" s="3" t="str">
         <f>[1]did_reg_emp!F30</f>
-        <v>0.193</v>
+        <v>0.198</v>
       </c>
       <c r="I25" s="3" t="str">
         <f>[1]did_reg_emp!G30</f>
-        <v>0.204</v>
+        <v>0.210</v>
       </c>
       <c r="K25" s="3" t="str">
         <f>[1]did_reg_emp!H30</f>
@@ -2195,29 +2195,29 @@
       </c>
       <c r="B26" s="10" t="str">
         <f>[1]did_reg_emp!B31</f>
-        <v>6.33</v>
+        <v>6.39</v>
       </c>
       <c r="C26" s="10" t="str">
         <f>[1]did_reg_emp!C31</f>
-        <v>6.32</v>
+        <v>6.38</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10" t="str">
         <f>[1]did_reg_emp!D31</f>
-        <v>3.18</v>
+        <v>3.21</v>
       </c>
       <c r="F26" s="10" t="str">
         <f>[1]did_reg_emp!E31</f>
-        <v>3.17</v>
+        <v>3.20</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10" t="str">
         <f>[1]did_reg_emp!F31</f>
-        <v>5.56</v>
+        <v>5.59</v>
       </c>
       <c r="I26" s="10" t="str">
         <f>[1]did_reg_emp!G31</f>
-        <v>5.55</v>
+        <v>5.58</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="str">
@@ -2257,7 +2257,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6">
         <f>ROUND([1]did_reg_emp!G33,3)</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>

</xml_diff>